<commit_message>
Code added for contraceptive (BIFAP)
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/ATC_lot4_formatted.xlsx
+++ b/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/ATC_lot4_formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://science.data.uu.nl/research-documents/Script development/Exchange Magda Ema/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpajo\Desktop\LOT4STUDIES\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{99EDEAC9-8AC7-43B7-BF3E-42D4F9B8390F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8960F354-AC9B-444C-BF63-EF0368DF690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valproate" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="351">
   <si>
     <t>Valproic acid</t>
   </si>
@@ -1083,12 +1083,18 @@
   </si>
   <si>
     <t>clindamycin/​benzoyl peroxide</t>
+  </si>
+  <si>
+    <t>G03HB01</t>
+  </si>
+  <si>
+    <t>Cyproterone acetate and ethinylestradiol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1596,7 +1602,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
@@ -1637,6 +1643,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1676,7 +1686,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1992,7 +2002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2060,11 +2070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2204,11 +2214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2494,13 +2504,28 @@
         <v>109</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="C19" t="s">
+        <v>350</v>
+      </c>
+      <c r="E19" t="s">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2674,7 +2699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2727,7 +2752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2780,7 +2805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2829,7 +2854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2878,11 +2903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,7 +3047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3099,7 +3124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3493,7 +3518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3619,7 +3644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3901,7 +3926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4710,7 +4735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5245,7 +5270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5599,7 +5624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
used codelist sent to BIFAP (in case error in previous commit/push)
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/ATC_lot4_formatted.xlsx
+++ b/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/ATC_lot4_formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31653\Desktop\LOT4_Sourcetree\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpajo\Desktop\LOT4STUDIES\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8ABA6DE-26D9-40E9-A22E-1BEA15711B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8960F354-AC9B-444C-BF63-EF0368DF690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valproate" sheetId="2" r:id="rId1"/>

</xml_diff>